<commit_message>
Update sample data for document extraction rules to include additional fields and extraction methods.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4d4c02d9-60b2-474c-ad6b-f5528ae0f4e8
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/2d21acb8-aeff-4051-b85a-bc5adb7a5bd7/ba73ca03-c9b9-4440-9bc1-4188c2325db4.jpg
</commit_message>
<xml_diff>
--- a/static/sample_extraction_rules.xlsx
+++ b/static/sample_extraction_rules.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,16 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>context_before</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>context_after</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>instructions</t>
         </is>
       </c>
@@ -471,21 +481,24 @@
           <t>after_pattern</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Extract text after Invoice # pattern</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total Amount</t>
+          <t>Invoice Date</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Total:</t>
+          <t>Invoice Date:</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -493,21 +506,24 @@
           <t>after_pattern</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Extract total amount from the invoice</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Customer Name</t>
+          <t>Total Amount</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bill To:</t>
+          <t>Total:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -515,34 +531,44 @@
           <t>after_pattern</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Extract customer name from billing information</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Shipping Address</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Company:</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nlp</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Find the full shipping address, including street, city, state and zip code</t>
-        </is>
-      </c>
+          <t>after_pattern</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Order Date</t>
+          <t>Customer Address</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -551,27 +577,71 @@
           <t>nlp</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Extract the date when the order was placed</t>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Find the complete customer address in the document</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Product Description</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>Customer Email</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Email:</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>regex</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Customer Support</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Phone:</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Payment Due Date</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>nlp</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Extract detailed description of the product including model number and specifications</t>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Extract the payment due date or deadline for payment</t>
         </is>
       </c>
     </row>

</xml_diff>